<commit_message>
assignment 2 log the file
</commit_message>
<xml_diff>
--- a/Employee_Personal_Details.xlsx
+++ b/Employee_Personal_Details.xlsx
@@ -462,39 +462,39 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>10761</v>
+        <v>61659</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Paige Carlson</t>
+          <t>Steven Nguyen</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>jessica85@example.org</t>
+          <t>iboyer@example.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>52798.72</v>
+        <v>69167.67</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>31733</v>
+        <v>1067</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Clinton Torres</t>
+          <t>Amanda Torres</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>iturner@example.org</t>
+          <t>lisa77@example.org</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -503,90 +503,90 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>60237.34</v>
+        <v>74755.39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>83927</v>
+        <v>77832</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Whitney Bradley</t>
+          <t>Susan Williams</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>turnerarthur@example.org</t>
+          <t>munozphillip@example.org</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>90087.71000000001</v>
+        <v>72115.27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>47307</v>
+        <v>19325</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Daniel Smith</t>
+          <t>Tiffany Mathews</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>donna20@example.net</t>
+          <t>travisclark@example.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>70577.82000000001</v>
+        <v>64673.01</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>43243</v>
+        <v>53246</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mrs. Jennifer Bray</t>
+          <t>Amy Boone</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>sarah52@example.net</t>
+          <t>sotojoseph@example.net</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>49603.7</v>
+        <v>97488.24000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>53894</v>
+        <v>69060</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Andrew Lynch</t>
+          <t>Gregory Delgado</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>icastro@example.org</t>
+          <t>erikrobles@example.org</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -595,44 +595,44 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>80872.85000000001</v>
+        <v>74642.62</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>55558</v>
+        <v>21824</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>James Phillips MD</t>
+          <t>Troy Jackson</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>brian72@example.net</t>
+          <t>alijames@example.org</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>30201.31</v>
+        <v>97886.82000000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>11027</v>
+        <v>77354</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jacqueline Tran</t>
+          <t>Alexis Morris</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>sara41@example.net</t>
+          <t>kimwillis@example.org</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -641,182 +641,182 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>45174.62</v>
+        <v>38066.89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>43737</v>
+        <v>92184</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Tammy Fletcher</t>
+          <t>Jessica Alexander</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>lesliecastillo@example.com</t>
+          <t>stephenhunt@example.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>79078.74000000001</v>
+        <v>78584.07000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>45637</v>
+        <v>80488</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Gregory Duncan</t>
+          <t>Nicole Barnett</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>pittmancurtis@example.org</t>
+          <t>kathrynbrewer@example.net</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>45495.03</v>
+        <v>92242.69</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>43011</v>
+        <v>59838</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Christine Kane</t>
+          <t>Danielle Stokes</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>carlos31@example.com</t>
+          <t>michael66@example.net</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>50147.42</v>
+        <v>33535.64</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>57821</v>
+        <v>23895</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Joshua Spencer</t>
+          <t>Daniel Parker</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>pollardgary@example.com</t>
+          <t>terry00@example.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>45423.14</v>
+        <v>64770.08</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>41254</v>
+        <v>49451</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Edward Bright</t>
+          <t>James Cruz</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>awhite@example.org</t>
+          <t>jacob86@example.com</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>98926.36</v>
+        <v>91037.25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>74994</v>
+        <v>88147</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Anna Stevens</t>
+          <t>John Lawrence</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>dkramer@example.net</t>
+          <t>williamsjessica@example.com</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>76823.47</v>
+        <v>62773.63</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>23222</v>
+        <v>75155</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>David Thomas</t>
+          <t>Christopher Taylor</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>jeffreygonzales@example.org</t>
+          <t>candace16@example.com</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>49594.52</v>
+        <v>73522.67999999999</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>61647</v>
+        <v>13759</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mr. Aaron Johnson</t>
+          <t>Briana Callahan</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>cynthia52@example.org</t>
+          <t>brendabrown@example.net</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -825,113 +825,113 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>78871.19</v>
+        <v>67722.32000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>33788</v>
+        <v>82142</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Heidi Saunders</t>
+          <t>Paul Davis</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>kylejacobson@example.com</t>
+          <t>qhaas@example.com</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>97957.10000000001</v>
+        <v>76547.41</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>49340</v>
+        <v>95753</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>David Craig</t>
+          <t>Pamela Schultz</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>jscott@example.net</t>
+          <t>aswanson@example.org</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>66999.64999999999</v>
+        <v>64147.81</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>82208</v>
+        <v>71361</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kevin Butler</t>
+          <t>Aaron Snyder</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>johnjohnson@example.net</t>
+          <t>alexis71@example.net</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>89391.36</v>
+        <v>51497.23</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>77976</v>
+        <v>17994</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kimberly Edwards</t>
+          <t>Courtney Jordan</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>john65@example.com</t>
+          <t>elizabethgillespie@example.org</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>58425.39</v>
+        <v>82466.96000000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>19885</v>
+        <v>78798</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Chelsea Taylor</t>
+          <t>Valerie Johnson</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>nicole14@example.com</t>
+          <t>wagnertracey@example.org</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -940,67 +940,67 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>47644.68</v>
+        <v>50435.27</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>79790</v>
+        <v>38804</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Casey Hicks</t>
+          <t>Brian Phillips</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>stewartdon@example.org</t>
+          <t>wmassey@example.net</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>44435.32</v>
+        <v>76496.41</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>38863</v>
+        <v>50540</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Justin Gonzales</t>
+          <t>Paula Henderson</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>eoconnor@example.com</t>
+          <t>smithcrystal@example.net</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>82280.48</v>
+        <v>55160.56</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>95001</v>
+        <v>45778</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Megan Hernandez</t>
+          <t>Christina Ponce</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>linda98@example.com</t>
+          <t>thomasbautista@example.org</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1009,21 +1009,21 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>82228.28</v>
+        <v>35877.29</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>68172</v>
+        <v>9855</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Martin Conner</t>
+          <t>Colton Ball</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>mitchellmcguire@example.com</t>
+          <t>ahicks@example.net</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1032,113 +1032,113 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>79675.73</v>
+        <v>48572.78</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>35248</v>
+        <v>83925</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Christina Montes</t>
+          <t>Kevin Diaz</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>hgutierrez@example.org</t>
+          <t>umcpherson@example.com</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>79533.85000000001</v>
+        <v>75219.74000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>31723</v>
+        <v>9983</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>David Tate</t>
+          <t>Tamara Diaz</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>joanguzman@example.com</t>
+          <t>mcfarlandkayla@example.com</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>68711.67</v>
+        <v>55072.3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>33749</v>
+        <v>96866</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Christopher Anderson</t>
+          <t>Timothy Malone</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>vmartinez@example.com</t>
+          <t>dyoung@example.net</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>52832.47</v>
+        <v>87109.81</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>26542</v>
+        <v>7240</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Joseph Green</t>
+          <t>Samuel Gilbert</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>qlopez@example.com</t>
+          <t>xgreen@example.com</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>84127.49000000001</v>
+        <v>97037.83</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>34746</v>
+        <v>41500</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Tara Mccoy</t>
+          <t>Scott Mosley</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>robin57@example.com</t>
+          <t>belljeanette@example.org</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1147,67 +1147,67 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>47644.98</v>
+        <v>66865.72</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>8305</v>
+        <v>95194</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Danny Baker</t>
+          <t>Michael Sanchez</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>heather74@example.net</t>
+          <t>brian22@example.org</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>79354.09</v>
+        <v>75863.83</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>28932</v>
+        <v>5528</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Timothy Bennett</t>
+          <t>Natalie Hobbs</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>edward52@example.net</t>
+          <t>tcampos@example.net</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>44350.77</v>
+        <v>69777.77</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>58890</v>
+        <v>81695</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Michael Whitaker</t>
+          <t>Robert Williamson</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>santanakeith@example.com</t>
+          <t>joseph09@example.org</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1216,21 +1216,21 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>58566.07</v>
+        <v>42403.21</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>49165</v>
+        <v>11207</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Ronald Kennedy</t>
+          <t>John Fox</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>lbauer@example.org</t>
+          <t>colemanmadison@example.com</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1239,21 +1239,21 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>50094.09</v>
+        <v>93745.14</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>22092</v>
+        <v>77409</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Lauren Franklin</t>
+          <t>Jason Robinson</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>jamesbrown@example.org</t>
+          <t>desireemartinez@example.net</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1262,44 +1262,44 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>91448.89</v>
+        <v>96146.98</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>61458</v>
+        <v>17129</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Charles Stewart</t>
+          <t>Courtney Atkins</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>timothy50@example.net</t>
+          <t>zwalker@example.com</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>63852.93</v>
+        <v>46623.77</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>41355</v>
+        <v>30597</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Angel Oneill</t>
+          <t>Gina Craig</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>valenzueladennis@example.com</t>
+          <t>elizabeth88@example.com</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1308,21 +1308,21 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>61868.63</v>
+        <v>85393.8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>5967</v>
+        <v>3506</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Richard Bird Jr.</t>
+          <t>Devon Perez</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>uhooper@example.com</t>
+          <t>williamsellers@example.net</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1331,205 +1331,205 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>59589.62</v>
+        <v>74333.44</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>88201</v>
+        <v>26501</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Kristina Elliott</t>
+          <t>Stephanie Shannon</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>johngonzalez@example.com</t>
+          <t>brianmassey@example.com</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>93803.60000000001</v>
+        <v>44799.56</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>95392</v>
+        <v>9802</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Stephanie Robbins</t>
+          <t>Stephanie Robinson</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>williamjackson@example.org</t>
+          <t>wolfemichael@example.org</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>97001.32000000001</v>
+        <v>87249.41</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>5403</v>
+        <v>86072</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Marc Thompson</t>
+          <t>Rachel Brown</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>adamsjose@example.com</t>
+          <t>sarah15@example.org</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>72024.03</v>
+        <v>85597.81</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>51103</v>
+        <v>78407</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Richard Hunter</t>
+          <t>David Oconnor</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>tracy09@example.net</t>
+          <t>bryanmorgan@example.net</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>93821.06</v>
+        <v>42880.66</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>13269</v>
+        <v>85645</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Aaron Cochran</t>
+          <t>Eric Harris</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>caseythomas@example.net</t>
+          <t>karen84@example.net</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>96915.21000000001</v>
+        <v>56804.75</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>56312</v>
+        <v>77525</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Robert Brown</t>
+          <t>Mrs. Taylor Morris</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>williamblanchard@example.org</t>
+          <t>taylorkimberly@example.net</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>91143.42</v>
+        <v>56055.9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>73131</v>
+        <v>30312</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Sheri Russo</t>
+          <t>Deborah Lara</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>wmorrison@example.org</t>
+          <t>mary84@example.net</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>57641.17</v>
+        <v>59789.99</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>55310</v>
+        <v>89256</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Rebecca Huerta</t>
+          <t>Kelly Ford</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>madison25@example.com</t>
+          <t>rwatson@example.net</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>84192.17999999999</v>
+        <v>88816.14</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>96585</v>
+        <v>99618</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Karen Hancock</t>
+          <t>Monique Edwards</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>alexis61@example.org</t>
+          <t>joshuagonzalez@example.com</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1538,44 +1538,44 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>76443.64999999999</v>
+        <v>81739.34</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>39953</v>
+        <v>64424</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Mackenzie Adams</t>
+          <t>Daniel Douglas</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>turnerpaul@example.com</t>
+          <t>everettcarlos@example.net</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>50989.67</v>
+        <v>44695.78</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>92281</v>
+        <v>84222</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Brandon Wilson</t>
+          <t>Jennifer Nelson</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>villalucas@example.com</t>
+          <t>millercaleb@example.net</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1584,7 +1584,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>66236.2</v>
+        <v>97034.64999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>